<commit_message>
add plot as requested
</commit_message>
<xml_diff>
--- a/config/model_inputs_demo.xlsx
+++ b/config/model_inputs_demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bmgf-my.sharepoint.com/personal/rui_han_gatesfoundation_org/Documents/Documents/GitHub/Ethiopia-HEP-Capacity-Analysis/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\PACE-HRH-UI\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{4D2B757C-B76C-4E63-AFF6-4E5FB6B83359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F21957F5-7A38-405E-98F2-26B417677D3E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37A1063-8038-46D1-A7FE-B2B50972AA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="830" firstSheet="8" activeTab="14" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="13400" tabRatio="830" firstSheet="1" activeTab="1" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="77" r:id="rId1"/>
@@ -312,7 +312,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="346">
   <si>
     <t>Pregnancy</t>
   </si>
@@ -1082,15 +1082,9 @@
     <t>Source:</t>
   </si>
   <si>
-    <t>TaskValues_basic</t>
-  </si>
-  <si>
     <t>TaskValues_expanded</t>
   </si>
   <si>
-    <t>Expanded</t>
-  </si>
-  <si>
     <t>Cells in green are imported directly into the model.</t>
   </si>
   <si>
@@ -1352,10 +1346,10 @@
     <t>StepCoverage</t>
   </si>
   <si>
-    <t>CoverageRates_step</t>
-  </si>
-  <si>
     <t>MaxUtilization</t>
+  </si>
+  <si>
+    <t>Demo</t>
   </si>
 </sst>
 </file>
@@ -2138,9 +2132,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2178,7 +2172,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2284,7 +2278,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2426,7 +2420,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2488,12 +2482,12 @@
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="P3" s="28" t="b">
         <v>1</v>
@@ -2507,7 +2501,7 @@
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="P4" s="28" t="b">
         <v>0</v>
@@ -2521,7 +2515,7 @@
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2589,7 +2583,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="16" customFormat="1" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="43" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>36</v>
@@ -2642,7 +2636,7 @@
     </row>
     <row r="2" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="52" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B2" s="53" t="s">
         <v>51</v>
@@ -2683,7 +2677,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>54</v>
@@ -2724,10 +2718,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C4" t="s">
         <v>151</v>
@@ -2766,10 +2760,10 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C5" t="s">
         <v>58</v>
@@ -2808,10 +2802,10 @@
     </row>
     <row r="6" spans="1:17" s="66" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="64" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C6" s="66" t="s">
         <v>60</v>
@@ -2850,10 +2844,10 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>56</v>
@@ -2874,7 +2868,7 @@
         <v>3.0680000000000001</v>
       </c>
       <c r="I7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="41"/>
@@ -2892,10 +2886,10 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>57</v>
@@ -2934,13 +2928,13 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>52</v>
@@ -2976,10 +2970,10 @@
     </row>
     <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C10" t="s">
         <v>154</v>
@@ -3018,13 +3012,13 @@
     </row>
     <row r="11" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="52" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B11" s="53" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D11" s="55" t="s">
         <v>52</v>
@@ -3042,13 +3036,13 @@
         <v>2.0927000000000001E-4</v>
       </c>
       <c r="I11" s="54" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J11" s="58">
         <v>4</v>
       </c>
       <c r="K11" s="54" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L11" s="58">
         <v>0.90986310592664843</v>
@@ -3064,13 +3058,13 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>52</v>
@@ -3094,7 +3088,7 @@
         <v>4</v>
       </c>
       <c r="K12" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L12" s="24">
         <v>1</v>
@@ -3110,10 +3104,10 @@
     </row>
     <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C13" t="s">
         <v>158</v>
@@ -3140,7 +3134,7 @@
         <v>0.05</v>
       </c>
       <c r="K13" s="41" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="L13" s="9">
         <v>1</v>
@@ -3156,10 +3150,10 @@
     </row>
     <row r="14" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="52" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B14" s="53" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C14" s="54" t="s">
         <v>155</v>
@@ -3198,10 +3192,10 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C15" t="s">
         <v>156</v>
@@ -3313,7 +3307,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="16" customFormat="1" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="43" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>36</v>
@@ -3366,7 +3360,7 @@
     </row>
     <row r="2" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="52" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B2" s="53" t="s">
         <v>51</v>
@@ -3407,7 +3401,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>54</v>
@@ -3448,10 +3442,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C4" t="s">
         <v>151</v>
@@ -3490,10 +3484,10 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C5" t="s">
         <v>58</v>
@@ -3532,10 +3526,10 @@
     </row>
     <row r="6" spans="1:17" s="66" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="64" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C6" s="66" t="s">
         <v>60</v>
@@ -3574,10 +3568,10 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>56</v>
@@ -3598,7 +3592,7 @@
         <v>3.0680000000000001</v>
       </c>
       <c r="I7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="41"/>
@@ -3616,10 +3610,10 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>57</v>
@@ -3658,13 +3652,13 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>52</v>
@@ -3700,10 +3694,10 @@
     </row>
     <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C10" t="s">
         <v>154</v>
@@ -3742,13 +3736,13 @@
     </row>
     <row r="11" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="52" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B11" s="53" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D11" s="55" t="s">
         <v>52</v>
@@ -3766,13 +3760,13 @@
         <v>2.0927000000000001E-4</v>
       </c>
       <c r="I11" s="54" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J11" s="58">
         <v>4</v>
       </c>
       <c r="K11" s="54" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L11" s="58">
         <v>0.90986310592664843</v>
@@ -3788,13 +3782,13 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>52</v>
@@ -3818,7 +3812,7 @@
         <v>4</v>
       </c>
       <c r="K12" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L12" s="24">
         <v>1</v>
@@ -3834,10 +3828,10 @@
     </row>
     <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C13" t="s">
         <v>158</v>
@@ -3864,7 +3858,7 @@
         <v>0.05</v>
       </c>
       <c r="K13" s="41" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="L13" s="9">
         <v>1</v>
@@ -3880,10 +3874,10 @@
     </row>
     <row r="14" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="52" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B14" s="53" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C14" s="54" t="s">
         <v>155</v>
@@ -3922,10 +3916,10 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C15" t="s">
         <v>156</v>
@@ -3964,10 +3958,10 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C16" t="s">
         <v>249</v>
@@ -4006,10 +4000,10 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C17" t="s">
         <v>250</v>
@@ -4048,10 +4042,10 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C18" t="s">
         <v>251</v>
@@ -4090,10 +4084,10 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C19" t="s">
         <v>252</v>
@@ -4132,10 +4126,10 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C20" t="s">
         <v>253</v>
@@ -4174,10 +4168,10 @@
     </row>
     <row r="21" spans="1:16" s="66" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="64" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C21" s="66" t="s">
         <v>254</v>
@@ -4216,10 +4210,10 @@
     </row>
     <row r="22" spans="1:16" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="52" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B22" s="53" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C22" s="54" t="s">
         <v>114</v>
@@ -4258,13 +4252,13 @@
     </row>
     <row r="23" spans="1:16" s="66" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="64" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B23" s="65" t="s">
         <v>149</v>
       </c>
       <c r="C23" s="66" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D23" s="67" t="s">
         <v>153</v>
@@ -4282,7 +4276,7 @@
         <v>1E-3</v>
       </c>
       <c r="I23" s="70" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J23" s="71"/>
       <c r="L23" s="71">
@@ -4384,67 +4378,67 @@
         <v>37</v>
       </c>
       <c r="C1" s="103" t="s">
+        <v>321</v>
+      </c>
+      <c r="D1" s="103" t="s">
+        <v>322</v>
+      </c>
+      <c r="E1" s="103" t="s">
         <v>323</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="F1" s="103" t="s">
         <v>324</v>
       </c>
-      <c r="E1" s="103" t="s">
+      <c r="G1" s="103" t="s">
         <v>325</v>
       </c>
-      <c r="F1" s="103" t="s">
+      <c r="H1" s="103" t="s">
         <v>326</v>
       </c>
-      <c r="G1" s="103" t="s">
+      <c r="I1" s="103" t="s">
         <v>327</v>
       </c>
-      <c r="H1" s="103" t="s">
+      <c r="J1" s="103" t="s">
         <v>328</v>
       </c>
-      <c r="I1" s="103" t="s">
+      <c r="K1" s="103" t="s">
         <v>329</v>
       </c>
-      <c r="J1" s="103" t="s">
+      <c r="L1" s="103" t="s">
         <v>330</v>
       </c>
-      <c r="K1" s="103" t="s">
+      <c r="M1" s="103" t="s">
         <v>331</v>
       </c>
-      <c r="L1" s="103" t="s">
+      <c r="N1" s="103" t="s">
         <v>332</v>
       </c>
-      <c r="M1" s="103" t="s">
+      <c r="O1" s="103" t="s">
         <v>333</v>
       </c>
-      <c r="N1" s="103" t="s">
+      <c r="P1" s="103" t="s">
         <v>334</v>
       </c>
-      <c r="O1" s="103" t="s">
+      <c r="Q1" s="103" t="s">
         <v>335</v>
       </c>
-      <c r="P1" s="103" t="s">
+      <c r="R1" s="103" t="s">
         <v>336</v>
       </c>
-      <c r="Q1" s="103" t="s">
+      <c r="S1" s="103" t="s">
         <v>337</v>
       </c>
-      <c r="R1" s="103" t="s">
+      <c r="T1" s="103" t="s">
         <v>338</v>
       </c>
-      <c r="S1" s="103" t="s">
+      <c r="U1" s="103" t="s">
         <v>339</v>
       </c>
-      <c r="T1" s="103" t="s">
+      <c r="V1" s="103" t="s">
         <v>340</v>
       </c>
-      <c r="U1" s="103" t="s">
+      <c r="W1" s="103" t="s">
         <v>341</v>
-      </c>
-      <c r="V1" s="103" t="s">
-        <v>342</v>
-      </c>
-      <c r="W1" s="103" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.35">
@@ -4592,7 +4586,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B4" t="s">
         <v>151</v>
@@ -4600,7 +4594,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B5" t="s">
         <v>58</v>
@@ -4608,7 +4602,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B6" t="s">
         <v>60</v>
@@ -4616,7 +4610,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B7" t="s">
         <v>56</v>
@@ -4624,7 +4618,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B8" t="s">
         <v>57</v>
@@ -4632,15 +4626,15 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B10" t="s">
         <v>154</v>
@@ -4648,23 +4642,23 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B13" t="s">
         <v>158</v>
@@ -4672,7 +4666,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B14" t="s">
         <v>155</v>
@@ -4680,7 +4674,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B15" t="s">
         <v>156</v>
@@ -4688,7 +4682,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B16" t="s">
         <v>249</v>
@@ -4711,7 +4705,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B17" t="s">
         <v>250</v>
@@ -4719,7 +4713,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B18" t="s">
         <v>251</v>
@@ -4727,7 +4721,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B19" t="s">
         <v>252</v>
@@ -4735,7 +4729,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B20" t="s">
         <v>253</v>
@@ -4743,7 +4737,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B21" t="s">
         <v>254</v>
@@ -4788,67 +4782,67 @@
         <v>37</v>
       </c>
       <c r="C1" s="103" t="s">
+        <v>321</v>
+      </c>
+      <c r="D1" s="103" t="s">
+        <v>322</v>
+      </c>
+      <c r="E1" s="103" t="s">
         <v>323</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="F1" s="103" t="s">
         <v>324</v>
       </c>
-      <c r="E1" s="103" t="s">
+      <c r="G1" s="103" t="s">
         <v>325</v>
       </c>
-      <c r="F1" s="103" t="s">
+      <c r="H1" s="103" t="s">
         <v>326</v>
       </c>
-      <c r="G1" s="103" t="s">
+      <c r="I1" s="103" t="s">
         <v>327</v>
       </c>
-      <c r="H1" s="103" t="s">
+      <c r="J1" s="103" t="s">
         <v>328</v>
       </c>
-      <c r="I1" s="103" t="s">
+      <c r="K1" s="103" t="s">
         <v>329</v>
       </c>
-      <c r="J1" s="103" t="s">
+      <c r="L1" s="103" t="s">
         <v>330</v>
       </c>
-      <c r="K1" s="103" t="s">
+      <c r="M1" s="103" t="s">
         <v>331</v>
       </c>
-      <c r="L1" s="103" t="s">
+      <c r="N1" s="103" t="s">
         <v>332</v>
       </c>
-      <c r="M1" s="103" t="s">
+      <c r="O1" s="103" t="s">
         <v>333</v>
       </c>
-      <c r="N1" s="103" t="s">
+      <c r="P1" s="103" t="s">
         <v>334</v>
       </c>
-      <c r="O1" s="103" t="s">
+      <c r="Q1" s="103" t="s">
         <v>335</v>
       </c>
-      <c r="P1" s="103" t="s">
+      <c r="R1" s="103" t="s">
         <v>336</v>
       </c>
-      <c r="Q1" s="103" t="s">
+      <c r="S1" s="103" t="s">
         <v>337</v>
       </c>
-      <c r="R1" s="103" t="s">
+      <c r="T1" s="103" t="s">
         <v>338</v>
       </c>
-      <c r="S1" s="103" t="s">
+      <c r="U1" s="103" t="s">
         <v>339</v>
       </c>
-      <c r="T1" s="103" t="s">
+      <c r="V1" s="103" t="s">
         <v>340</v>
       </c>
-      <c r="U1" s="103" t="s">
+      <c r="W1" s="103" t="s">
         <v>341</v>
-      </c>
-      <c r="V1" s="103" t="s">
-        <v>342</v>
-      </c>
-      <c r="W1" s="103" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.35">
@@ -4872,7 +4866,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B4" t="s">
         <v>151</v>
@@ -4880,7 +4874,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B5" t="s">
         <v>58</v>
@@ -4888,7 +4882,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B6" t="s">
         <v>60</v>
@@ -4896,7 +4890,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B7" t="s">
         <v>56</v>
@@ -4904,7 +4898,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B8" t="s">
         <v>57</v>
@@ -4912,15 +4906,15 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B10" t="s">
         <v>154</v>
@@ -4928,23 +4922,23 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B13" t="s">
         <v>158</v>
@@ -4952,7 +4946,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B14" t="s">
         <v>155</v>
@@ -4960,7 +4954,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B15" t="s">
         <v>156</v>
@@ -4968,7 +4962,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B16" t="s">
         <v>249</v>
@@ -4976,7 +4970,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B17" t="s">
         <v>250</v>
@@ -4984,7 +4978,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B18" t="s">
         <v>251</v>
@@ -4992,7 +4986,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B19" t="s">
         <v>252</v>
@@ -5000,7 +4994,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B20" t="s">
         <v>253</v>
@@ -5008,7 +5002,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B21" t="s">
         <v>254</v>
@@ -5055,10 +5049,10 @@
   <sheetData>
     <row r="1" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="85" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B1" s="87" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C1" s="88" t="str">
         <f>_xlfn.CONCAT("StartYear", 2020)</f>
@@ -5125,43 +5119,43 @@
         <v>37</v>
       </c>
       <c r="C2" s="90" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D2" s="90" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E2" s="91" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="90" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G2" s="90" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H2" s="91" t="s">
         <v>34</v>
       </c>
       <c r="I2" s="90" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J2" s="90" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K2" s="90" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="L2" s="91" t="s">
         <v>34</v>
       </c>
       <c r="M2" s="90" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="N2" s="90" t="s">
+        <v>302</v>
+      </c>
+      <c r="O2" s="90" t="s">
         <v>304</v>
-      </c>
-      <c r="O2" s="90" t="s">
-        <v>306</v>
       </c>
       <c r="P2" s="91" t="s">
         <v>34</v>
@@ -5279,7 +5273,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="37" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B5" t="str">
         <f>VLOOKUP(A5,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5334,7 +5328,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="37" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B6" t="str">
         <f>VLOOKUP(A6,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5389,7 +5383,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B7" t="str">
         <f>VLOOKUP(A7,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5444,7 +5438,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B8" t="str">
         <f>VLOOKUP(A8,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5499,7 +5493,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="37" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B9" t="str">
         <f>VLOOKUP(A9,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5554,7 +5548,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="37" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B10" t="str">
         <f>VLOOKUP(A10,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5609,7 +5603,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="37" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B11" t="str">
         <f>VLOOKUP(A11,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5664,7 +5658,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="37" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B12" t="str">
         <f>VLOOKUP(A12,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5719,7 +5713,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="37" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B13" t="str">
         <f>VLOOKUP(A13,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5774,7 +5768,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="37" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B14" t="str">
         <f>VLOOKUP(A14,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5829,7 +5823,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="37" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B15" t="str">
         <f>VLOOKUP(A15,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5884,7 +5878,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="37" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B16" t="str">
         <f>VLOOKUP(A16,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5939,7 +5933,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B17" t="str">
         <f>VLOOKUP(A17,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5994,7 +5988,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B18" t="str">
         <f>VLOOKUP(A18,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -6049,7 +6043,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B19" t="str">
         <f>VLOOKUP(A19,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -6104,7 +6098,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B20" t="str">
         <f>VLOOKUP(A20,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -6159,7 +6153,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B21" t="str">
         <f>VLOOKUP(A21,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -6214,7 +6208,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B22" t="str">
         <f>VLOOKUP(A22,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -6269,7 +6263,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B23" t="str">
         <f>VLOOKUP(A23,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -6413,8 +6407,8 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6429,16 +6423,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="82" t="s">
+        <v>298</v>
+      </c>
+      <c r="B1" s="82" t="s">
+        <v>299</v>
+      </c>
+      <c r="C1" s="82" t="s">
         <v>300</v>
       </c>
-      <c r="B1" s="82" t="s">
-        <v>301</v>
-      </c>
-      <c r="C1" s="82" t="s">
-        <v>302</v>
-      </c>
       <c r="D1" s="82" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E1" s="82" t="s">
         <v>247</v>
@@ -6449,13 +6443,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D2" s="22">
         <v>5</v>
@@ -6469,13 +6463,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D3" s="22">
         <v>5</v>
@@ -6487,13 +6481,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D4" s="22">
         <v>5</v>
@@ -6505,13 +6499,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>258</v>
+        <v>345</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D5" s="22">
         <v>5</v>
@@ -6525,13 +6519,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>258</v>
+        <v>345</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D6" s="22">
         <v>5</v>
@@ -6543,13 +6537,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>258</v>
+        <v>345</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D7" s="22">
         <v>5</v>
@@ -6561,13 +6555,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D8" s="22">
         <v>5</v>
@@ -6581,13 +6575,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D9" s="22">
         <v>5</v>
@@ -6599,13 +6593,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D10" s="22">
         <v>5</v>
@@ -6617,13 +6611,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D11" s="22">
         <v>5</v>
@@ -6637,13 +6631,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D12" s="22">
         <v>5</v>
@@ -6655,13 +6649,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D13" s="22">
         <v>5</v>
@@ -6873,7 +6867,7 @@
         <v>176</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
@@ -6899,7 +6893,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.35">
@@ -6925,7 +6919,7 @@
         <v>4</v>
       </c>
       <c r="L3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
@@ -6951,7 +6945,7 @@
         <v>9</v>
       </c>
       <c r="L4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -6977,7 +6971,7 @@
         <v>9</v>
       </c>
       <c r="L5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
@@ -7956,10 +7950,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7989,7 +7983,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="83" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="E1" s="83" t="s">
         <v>9</v>
@@ -8019,12 +8013,12 @@
         <v>170</v>
       </c>
       <c r="N1" s="83" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
-        <v>298</v>
+      <c r="A2" s="5" t="s">
+        <v>345</v>
       </c>
       <c r="B2" s="27">
         <v>48</v>
@@ -8054,149 +8048,48 @@
         <v>256</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>143</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="B3" s="27">
-        <v>48</v>
-      </c>
-      <c r="C3" s="27">
-        <v>32</v>
-      </c>
-      <c r="D3" s="27">
-        <v>0.85</v>
-      </c>
-      <c r="E3" s="27">
-        <v>5000</v>
-      </c>
-      <c r="F3" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>344</v>
-      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="B4" s="27">
-        <v>48</v>
-      </c>
-      <c r="C4" s="27">
-        <v>32</v>
-      </c>
-      <c r="D4" s="27">
-        <v>0.85</v>
-      </c>
-      <c r="E4" s="27">
-        <v>5000</v>
-      </c>
-      <c r="F4" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>344</v>
-      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="B5" s="27">
-        <v>48</v>
-      </c>
-      <c r="C5" s="27">
-        <v>32</v>
-      </c>
-      <c r="D5" s="27">
-        <v>0.85</v>
-      </c>
-      <c r="E5" s="27">
-        <v>5000</v>
-      </c>
-      <c r="F5" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>346</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B6" s="4"/>
@@ -8218,44 +8111,13 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C4 E2:E4" xr:uid="{51E01DD3-1F4F-4ECB-945C-BF7AC154B4D2}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C2 E2" xr:uid="{51E01DD3-1F4F-4ECB-945C-BF7AC154B4D2}">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A5 J2:M4 J5" xr:uid="{87300A30-10E8-4D88-9E37-E7127D8D74E3}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:M2 A2" xr:uid="{87300A30-10E8-4D88-9E37-E7127D8D74E3}">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -8273,7 +8135,7 @@
           <x14:formula1>
             <xm:f>'Read Me'!$P$3:$P$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:I4</xm:sqref>
+          <xm:sqref>F2:I2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8335,7 +8197,7 @@
         <v>179</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>180</v>
@@ -8361,7 +8223,7 @@
         <v>181</v>
       </c>
       <c r="B3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>180</v>
@@ -8569,7 +8431,7 @@
         <v>189</v>
       </c>
       <c r="B11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>180</v>
@@ -9163,13 +9025,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="92" t="s">
+        <v>314</v>
+      </c>
+      <c r="B1" s="93" t="s">
+        <v>315</v>
+      </c>
+      <c r="C1" s="94" t="s">
         <v>316</v>
-      </c>
-      <c r="B1" s="93" t="s">
-        <v>317</v>
-      </c>
-      <c r="C1" s="94" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -9196,7 +9058,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="100" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B4" s="101"/>
       <c r="C4" s="102"/>
@@ -12537,7 +12399,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B3" t="s">
         <v>58</v>
@@ -12562,7 +12424,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B4" t="s">
         <v>60</v>
@@ -12581,7 +12443,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B5" t="s">
         <v>151</v>
@@ -12604,7 +12466,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B6" t="s">
         <v>150</v>
@@ -12625,7 +12487,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B7" t="s">
         <v>155</v>
@@ -12644,7 +12506,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B8" t="s">
         <v>156</v>
@@ -12663,7 +12525,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B9" t="s">
         <v>157</v>

</xml_diff>

<commit_message>
add plot as requested (#37)
* add plot as requested

* Add cadre roles plot

Add hours by cadre roles plot

---------

Co-authored-by: Rui Han <rui.han@gatesfoundation.org>
</commit_message>
<xml_diff>
--- a/config/model_inputs_demo.xlsx
+++ b/config/model_inputs_demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bmgf-my.sharepoint.com/personal/rui_han_gatesfoundation_org/Documents/Documents/GitHub/Ethiopia-HEP-Capacity-Analysis/config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\PACE-HRH-UI\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{4D2B757C-B76C-4E63-AFF6-4E5FB6B83359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F21957F5-7A38-405E-98F2-26B417677D3E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37A1063-8038-46D1-A7FE-B2B50972AA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="830" firstSheet="8" activeTab="14" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="13400" tabRatio="830" firstSheet="1" activeTab="1" xr2:uid="{2F49C92C-A2E5-4A6B-9429-02A43E12B5B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="77" r:id="rId1"/>
@@ -312,7 +312,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="346">
   <si>
     <t>Pregnancy</t>
   </si>
@@ -1082,15 +1082,9 @@
     <t>Source:</t>
   </si>
   <si>
-    <t>TaskValues_basic</t>
-  </si>
-  <si>
     <t>TaskValues_expanded</t>
   </si>
   <si>
-    <t>Expanded</t>
-  </si>
-  <si>
     <t>Cells in green are imported directly into the model.</t>
   </si>
   <si>
@@ -1352,10 +1346,10 @@
     <t>StepCoverage</t>
   </si>
   <si>
-    <t>CoverageRates_step</t>
-  </si>
-  <si>
     <t>MaxUtilization</t>
+  </si>
+  <si>
+    <t>Demo</t>
   </si>
 </sst>
 </file>
@@ -2138,9 +2132,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2178,7 +2172,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2284,7 +2278,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2426,7 +2420,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2488,12 +2482,12 @@
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="P3" s="28" t="b">
         <v>1</v>
@@ -2507,7 +2501,7 @@
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="P4" s="28" t="b">
         <v>0</v>
@@ -2521,7 +2515,7 @@
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2589,7 +2583,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="16" customFormat="1" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="43" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>36</v>
@@ -2642,7 +2636,7 @@
     </row>
     <row r="2" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="52" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B2" s="53" t="s">
         <v>51</v>
@@ -2683,7 +2677,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>54</v>
@@ -2724,10 +2718,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C4" t="s">
         <v>151</v>
@@ -2766,10 +2760,10 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C5" t="s">
         <v>58</v>
@@ -2808,10 +2802,10 @@
     </row>
     <row r="6" spans="1:17" s="66" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="64" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C6" s="66" t="s">
         <v>60</v>
@@ -2850,10 +2844,10 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>56</v>
@@ -2874,7 +2868,7 @@
         <v>3.0680000000000001</v>
       </c>
       <c r="I7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="41"/>
@@ -2892,10 +2886,10 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>57</v>
@@ -2934,13 +2928,13 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>52</v>
@@ -2976,10 +2970,10 @@
     </row>
     <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C10" t="s">
         <v>154</v>
@@ -3018,13 +3012,13 @@
     </row>
     <row r="11" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="52" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B11" s="53" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D11" s="55" t="s">
         <v>52</v>
@@ -3042,13 +3036,13 @@
         <v>2.0927000000000001E-4</v>
       </c>
       <c r="I11" s="54" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J11" s="58">
         <v>4</v>
       </c>
       <c r="K11" s="54" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L11" s="58">
         <v>0.90986310592664843</v>
@@ -3064,13 +3058,13 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>52</v>
@@ -3094,7 +3088,7 @@
         <v>4</v>
       </c>
       <c r="K12" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L12" s="24">
         <v>1</v>
@@ -3110,10 +3104,10 @@
     </row>
     <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C13" t="s">
         <v>158</v>
@@ -3140,7 +3134,7 @@
         <v>0.05</v>
       </c>
       <c r="K13" s="41" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="L13" s="9">
         <v>1</v>
@@ -3156,10 +3150,10 @@
     </row>
     <row r="14" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="52" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B14" s="53" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C14" s="54" t="s">
         <v>155</v>
@@ -3198,10 +3192,10 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C15" t="s">
         <v>156</v>
@@ -3313,7 +3307,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="16" customFormat="1" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="43" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>36</v>
@@ -3366,7 +3360,7 @@
     </row>
     <row r="2" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="52" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B2" s="53" t="s">
         <v>51</v>
@@ -3407,7 +3401,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>54</v>
@@ -3448,10 +3442,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C4" t="s">
         <v>151</v>
@@ -3490,10 +3484,10 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C5" t="s">
         <v>58</v>
@@ -3532,10 +3526,10 @@
     </row>
     <row r="6" spans="1:17" s="66" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="64" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C6" s="66" t="s">
         <v>60</v>
@@ -3574,10 +3568,10 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>56</v>
@@ -3598,7 +3592,7 @@
         <v>3.0680000000000001</v>
       </c>
       <c r="I7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="41"/>
@@ -3616,10 +3610,10 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>57</v>
@@ -3658,13 +3652,13 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>52</v>
@@ -3700,10 +3694,10 @@
     </row>
     <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C10" t="s">
         <v>154</v>
@@ -3742,13 +3736,13 @@
     </row>
     <row r="11" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="52" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B11" s="53" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D11" s="55" t="s">
         <v>52</v>
@@ -3766,13 +3760,13 @@
         <v>2.0927000000000001E-4</v>
       </c>
       <c r="I11" s="54" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J11" s="58">
         <v>4</v>
       </c>
       <c r="K11" s="54" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L11" s="58">
         <v>0.90986310592664843</v>
@@ -3788,13 +3782,13 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>52</v>
@@ -3818,7 +3812,7 @@
         <v>4</v>
       </c>
       <c r="K12" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L12" s="24">
         <v>1</v>
@@ -3834,10 +3828,10 @@
     </row>
     <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C13" t="s">
         <v>158</v>
@@ -3864,7 +3858,7 @@
         <v>0.05</v>
       </c>
       <c r="K13" s="41" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="L13" s="9">
         <v>1</v>
@@ -3880,10 +3874,10 @@
     </row>
     <row r="14" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="52" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B14" s="53" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C14" s="54" t="s">
         <v>155</v>
@@ -3922,10 +3916,10 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C15" t="s">
         <v>156</v>
@@ -3964,10 +3958,10 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C16" t="s">
         <v>249</v>
@@ -4006,10 +4000,10 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C17" t="s">
         <v>250</v>
@@ -4048,10 +4042,10 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C18" t="s">
         <v>251</v>
@@ -4090,10 +4084,10 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C19" t="s">
         <v>252</v>
@@ -4132,10 +4126,10 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C20" t="s">
         <v>253</v>
@@ -4174,10 +4168,10 @@
     </row>
     <row r="21" spans="1:16" s="66" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="64" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C21" s="66" t="s">
         <v>254</v>
@@ -4216,10 +4210,10 @@
     </row>
     <row r="22" spans="1:16" s="54" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="52" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B22" s="53" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C22" s="54" t="s">
         <v>114</v>
@@ -4258,13 +4252,13 @@
     </row>
     <row r="23" spans="1:16" s="66" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="64" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B23" s="65" t="s">
         <v>149</v>
       </c>
       <c r="C23" s="66" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D23" s="67" t="s">
         <v>153</v>
@@ -4282,7 +4276,7 @@
         <v>1E-3</v>
       </c>
       <c r="I23" s="70" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J23" s="71"/>
       <c r="L23" s="71">
@@ -4384,67 +4378,67 @@
         <v>37</v>
       </c>
       <c r="C1" s="103" t="s">
+        <v>321</v>
+      </c>
+      <c r="D1" s="103" t="s">
+        <v>322</v>
+      </c>
+      <c r="E1" s="103" t="s">
         <v>323</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="F1" s="103" t="s">
         <v>324</v>
       </c>
-      <c r="E1" s="103" t="s">
+      <c r="G1" s="103" t="s">
         <v>325</v>
       </c>
-      <c r="F1" s="103" t="s">
+      <c r="H1" s="103" t="s">
         <v>326</v>
       </c>
-      <c r="G1" s="103" t="s">
+      <c r="I1" s="103" t="s">
         <v>327</v>
       </c>
-      <c r="H1" s="103" t="s">
+      <c r="J1" s="103" t="s">
         <v>328</v>
       </c>
-      <c r="I1" s="103" t="s">
+      <c r="K1" s="103" t="s">
         <v>329</v>
       </c>
-      <c r="J1" s="103" t="s">
+      <c r="L1" s="103" t="s">
         <v>330</v>
       </c>
-      <c r="K1" s="103" t="s">
+      <c r="M1" s="103" t="s">
         <v>331</v>
       </c>
-      <c r="L1" s="103" t="s">
+      <c r="N1" s="103" t="s">
         <v>332</v>
       </c>
-      <c r="M1" s="103" t="s">
+      <c r="O1" s="103" t="s">
         <v>333</v>
       </c>
-      <c r="N1" s="103" t="s">
+      <c r="P1" s="103" t="s">
         <v>334</v>
       </c>
-      <c r="O1" s="103" t="s">
+      <c r="Q1" s="103" t="s">
         <v>335</v>
       </c>
-      <c r="P1" s="103" t="s">
+      <c r="R1" s="103" t="s">
         <v>336</v>
       </c>
-      <c r="Q1" s="103" t="s">
+      <c r="S1" s="103" t="s">
         <v>337</v>
       </c>
-      <c r="R1" s="103" t="s">
+      <c r="T1" s="103" t="s">
         <v>338</v>
       </c>
-      <c r="S1" s="103" t="s">
+      <c r="U1" s="103" t="s">
         <v>339</v>
       </c>
-      <c r="T1" s="103" t="s">
+      <c r="V1" s="103" t="s">
         <v>340</v>
       </c>
-      <c r="U1" s="103" t="s">
+      <c r="W1" s="103" t="s">
         <v>341</v>
-      </c>
-      <c r="V1" s="103" t="s">
-        <v>342</v>
-      </c>
-      <c r="W1" s="103" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.35">
@@ -4592,7 +4586,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B4" t="s">
         <v>151</v>
@@ -4600,7 +4594,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B5" t="s">
         <v>58</v>
@@ -4608,7 +4602,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B6" t="s">
         <v>60</v>
@@ -4616,7 +4610,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B7" t="s">
         <v>56</v>
@@ -4624,7 +4618,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B8" t="s">
         <v>57</v>
@@ -4632,15 +4626,15 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B10" t="s">
         <v>154</v>
@@ -4648,23 +4642,23 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B13" t="s">
         <v>158</v>
@@ -4672,7 +4666,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B14" t="s">
         <v>155</v>
@@ -4680,7 +4674,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B15" t="s">
         <v>156</v>
@@ -4688,7 +4682,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B16" t="s">
         <v>249</v>
@@ -4711,7 +4705,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B17" t="s">
         <v>250</v>
@@ -4719,7 +4713,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B18" t="s">
         <v>251</v>
@@ -4727,7 +4721,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B19" t="s">
         <v>252</v>
@@ -4735,7 +4729,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B20" t="s">
         <v>253</v>
@@ -4743,7 +4737,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B21" t="s">
         <v>254</v>
@@ -4788,67 +4782,67 @@
         <v>37</v>
       </c>
       <c r="C1" s="103" t="s">
+        <v>321</v>
+      </c>
+      <c r="D1" s="103" t="s">
+        <v>322</v>
+      </c>
+      <c r="E1" s="103" t="s">
         <v>323</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="F1" s="103" t="s">
         <v>324</v>
       </c>
-      <c r="E1" s="103" t="s">
+      <c r="G1" s="103" t="s">
         <v>325</v>
       </c>
-      <c r="F1" s="103" t="s">
+      <c r="H1" s="103" t="s">
         <v>326</v>
       </c>
-      <c r="G1" s="103" t="s">
+      <c r="I1" s="103" t="s">
         <v>327</v>
       </c>
-      <c r="H1" s="103" t="s">
+      <c r="J1" s="103" t="s">
         <v>328</v>
       </c>
-      <c r="I1" s="103" t="s">
+      <c r="K1" s="103" t="s">
         <v>329</v>
       </c>
-      <c r="J1" s="103" t="s">
+      <c r="L1" s="103" t="s">
         <v>330</v>
       </c>
-      <c r="K1" s="103" t="s">
+      <c r="M1" s="103" t="s">
         <v>331</v>
       </c>
-      <c r="L1" s="103" t="s">
+      <c r="N1" s="103" t="s">
         <v>332</v>
       </c>
-      <c r="M1" s="103" t="s">
+      <c r="O1" s="103" t="s">
         <v>333</v>
       </c>
-      <c r="N1" s="103" t="s">
+      <c r="P1" s="103" t="s">
         <v>334</v>
       </c>
-      <c r="O1" s="103" t="s">
+      <c r="Q1" s="103" t="s">
         <v>335</v>
       </c>
-      <c r="P1" s="103" t="s">
+      <c r="R1" s="103" t="s">
         <v>336</v>
       </c>
-      <c r="Q1" s="103" t="s">
+      <c r="S1" s="103" t="s">
         <v>337</v>
       </c>
-      <c r="R1" s="103" t="s">
+      <c r="T1" s="103" t="s">
         <v>338</v>
       </c>
-      <c r="S1" s="103" t="s">
+      <c r="U1" s="103" t="s">
         <v>339</v>
       </c>
-      <c r="T1" s="103" t="s">
+      <c r="V1" s="103" t="s">
         <v>340</v>
       </c>
-      <c r="U1" s="103" t="s">
+      <c r="W1" s="103" t="s">
         <v>341</v>
-      </c>
-      <c r="V1" s="103" t="s">
-        <v>342</v>
-      </c>
-      <c r="W1" s="103" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.35">
@@ -4872,7 +4866,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B4" t="s">
         <v>151</v>
@@ -4880,7 +4874,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B5" t="s">
         <v>58</v>
@@ -4888,7 +4882,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B6" t="s">
         <v>60</v>
@@ -4896,7 +4890,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B7" t="s">
         <v>56</v>
@@ -4904,7 +4898,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B8" t="s">
         <v>57</v>
@@ -4912,15 +4906,15 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B10" t="s">
         <v>154</v>
@@ -4928,23 +4922,23 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B13" t="s">
         <v>158</v>
@@ -4952,7 +4946,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B14" t="s">
         <v>155</v>
@@ -4960,7 +4954,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B15" t="s">
         <v>156</v>
@@ -4968,7 +4962,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B16" t="s">
         <v>249</v>
@@ -4976,7 +4970,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B17" t="s">
         <v>250</v>
@@ -4984,7 +4978,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B18" t="s">
         <v>251</v>
@@ -4992,7 +4986,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B19" t="s">
         <v>252</v>
@@ -5000,7 +4994,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B20" t="s">
         <v>253</v>
@@ -5008,7 +5002,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B21" t="s">
         <v>254</v>
@@ -5055,10 +5049,10 @@
   <sheetData>
     <row r="1" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="85" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B1" s="87" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C1" s="88" t="str">
         <f>_xlfn.CONCAT("StartYear", 2020)</f>
@@ -5125,43 +5119,43 @@
         <v>37</v>
       </c>
       <c r="C2" s="90" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D2" s="90" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E2" s="91" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="90" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G2" s="90" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H2" s="91" t="s">
         <v>34</v>
       </c>
       <c r="I2" s="90" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J2" s="90" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K2" s="90" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="L2" s="91" t="s">
         <v>34</v>
       </c>
       <c r="M2" s="90" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="N2" s="90" t="s">
+        <v>302</v>
+      </c>
+      <c r="O2" s="90" t="s">
         <v>304</v>
-      </c>
-      <c r="O2" s="90" t="s">
-        <v>306</v>
       </c>
       <c r="P2" s="91" t="s">
         <v>34</v>
@@ -5279,7 +5273,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="37" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B5" t="str">
         <f>VLOOKUP(A5,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5334,7 +5328,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="37" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B6" t="str">
         <f>VLOOKUP(A6,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5389,7 +5383,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B7" t="str">
         <f>VLOOKUP(A7,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5444,7 +5438,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B8" t="str">
         <f>VLOOKUP(A8,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5499,7 +5493,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="37" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B9" t="str">
         <f>VLOOKUP(A9,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5554,7 +5548,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="37" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B10" t="str">
         <f>VLOOKUP(A10,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5609,7 +5603,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="37" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B11" t="str">
         <f>VLOOKUP(A11,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5664,7 +5658,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="37" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B12" t="str">
         <f>VLOOKUP(A12,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5719,7 +5713,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="37" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B13" t="str">
         <f>VLOOKUP(A13,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5774,7 +5768,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="37" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B14" t="str">
         <f>VLOOKUP(A14,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5829,7 +5823,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="37" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B15" t="str">
         <f>VLOOKUP(A15,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5884,7 +5878,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="37" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B16" t="str">
         <f>VLOOKUP(A16,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5939,7 +5933,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B17" t="str">
         <f>VLOOKUP(A17,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -5994,7 +5988,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B18" t="str">
         <f>VLOOKUP(A18,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -6049,7 +6043,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B19" t="str">
         <f>VLOOKUP(A19,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -6104,7 +6098,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B20" t="str">
         <f>VLOOKUP(A20,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -6159,7 +6153,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B21" t="str">
         <f>VLOOKUP(A21,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -6214,7 +6208,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B22" t="str">
         <f>VLOOKUP(A22,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -6269,7 +6263,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B23" t="str">
         <f>VLOOKUP(A23,TaskValues_expanded!B:C,2,FALSE)</f>
@@ -6413,8 +6407,8 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6429,16 +6423,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="82" t="s">
+        <v>298</v>
+      </c>
+      <c r="B1" s="82" t="s">
+        <v>299</v>
+      </c>
+      <c r="C1" s="82" t="s">
         <v>300</v>
       </c>
-      <c r="B1" s="82" t="s">
-        <v>301</v>
-      </c>
-      <c r="C1" s="82" t="s">
-        <v>302</v>
-      </c>
       <c r="D1" s="82" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E1" s="82" t="s">
         <v>247</v>
@@ -6449,13 +6443,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D2" s="22">
         <v>5</v>
@@ -6469,13 +6463,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D3" s="22">
         <v>5</v>
@@ -6487,13 +6481,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D4" s="22">
         <v>5</v>
@@ -6505,13 +6499,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>258</v>
+        <v>345</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D5" s="22">
         <v>5</v>
@@ -6525,13 +6519,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>258</v>
+        <v>345</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D6" s="22">
         <v>5</v>
@@ -6543,13 +6537,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>258</v>
+        <v>345</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D7" s="22">
         <v>5</v>
@@ -6561,13 +6555,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D8" s="22">
         <v>5</v>
@@ -6581,13 +6575,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D9" s="22">
         <v>5</v>
@@ -6599,13 +6593,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D10" s="22">
         <v>5</v>
@@ -6617,13 +6611,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D11" s="22">
         <v>5</v>
@@ -6637,13 +6631,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D12" s="22">
         <v>5</v>
@@ -6655,13 +6649,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D13" s="22">
         <v>5</v>
@@ -6873,7 +6867,7 @@
         <v>176</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
@@ -6899,7 +6893,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.35">
@@ -6925,7 +6919,7 @@
         <v>4</v>
       </c>
       <c r="L3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
@@ -6951,7 +6945,7 @@
         <v>9</v>
       </c>
       <c r="L4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -6977,7 +6971,7 @@
         <v>9</v>
       </c>
       <c r="L5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
@@ -7956,10 +7950,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7989,7 +7983,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="83" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="E1" s="83" t="s">
         <v>9</v>
@@ -8019,12 +8013,12 @@
         <v>170</v>
       </c>
       <c r="N1" s="83" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
-        <v>298</v>
+      <c r="A2" s="5" t="s">
+        <v>345</v>
       </c>
       <c r="B2" s="27">
         <v>48</v>
@@ -8054,149 +8048,48 @@
         <v>256</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>143</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="B3" s="27">
-        <v>48</v>
-      </c>
-      <c r="C3" s="27">
-        <v>32</v>
-      </c>
-      <c r="D3" s="27">
-        <v>0.85</v>
-      </c>
-      <c r="E3" s="27">
-        <v>5000</v>
-      </c>
-      <c r="F3" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>344</v>
-      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="B4" s="27">
-        <v>48</v>
-      </c>
-      <c r="C4" s="27">
-        <v>32</v>
-      </c>
-      <c r="D4" s="27">
-        <v>0.85</v>
-      </c>
-      <c r="E4" s="27">
-        <v>5000</v>
-      </c>
-      <c r="F4" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>344</v>
-      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="B5" s="27">
-        <v>48</v>
-      </c>
-      <c r="C5" s="27">
-        <v>32</v>
-      </c>
-      <c r="D5" s="27">
-        <v>0.85</v>
-      </c>
-      <c r="E5" s="27">
-        <v>5000</v>
-      </c>
-      <c r="F5" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>346</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B6" s="4"/>
@@ -8218,44 +8111,13 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C4 E2:E4" xr:uid="{51E01DD3-1F4F-4ECB-945C-BF7AC154B4D2}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C2 E2" xr:uid="{51E01DD3-1F4F-4ECB-945C-BF7AC154B4D2}">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A5 J2:M4 J5" xr:uid="{87300A30-10E8-4D88-9E37-E7127D8D74E3}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:M2 A2" xr:uid="{87300A30-10E8-4D88-9E37-E7127D8D74E3}">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -8273,7 +8135,7 @@
           <x14:formula1>
             <xm:f>'Read Me'!$P$3:$P$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:I4</xm:sqref>
+          <xm:sqref>F2:I2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8335,7 +8197,7 @@
         <v>179</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>180</v>
@@ -8361,7 +8223,7 @@
         <v>181</v>
       </c>
       <c r="B3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>180</v>
@@ -8569,7 +8431,7 @@
         <v>189</v>
       </c>
       <c r="B11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>180</v>
@@ -9163,13 +9025,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="92" t="s">
+        <v>314</v>
+      </c>
+      <c r="B1" s="93" t="s">
+        <v>315</v>
+      </c>
+      <c r="C1" s="94" t="s">
         <v>316</v>
-      </c>
-      <c r="B1" s="93" t="s">
-        <v>317</v>
-      </c>
-      <c r="C1" s="94" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -9196,7 +9058,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="100" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B4" s="101"/>
       <c r="C4" s="102"/>
@@ -12537,7 +12399,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B3" t="s">
         <v>58</v>
@@ -12562,7 +12424,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B4" t="s">
         <v>60</v>
@@ -12581,7 +12443,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B5" t="s">
         <v>151</v>
@@ -12604,7 +12466,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B6" t="s">
         <v>150</v>
@@ -12625,7 +12487,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B7" t="s">
         <v>155</v>
@@ -12644,7 +12506,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B8" t="s">
         <v>156</v>
@@ -12663,7 +12525,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B9" t="s">
         <v>157</v>

</xml_diff>